<commit_message>
Fix formula error in new green hydrogen electricity capacity logit function, calibrate logit parameters
</commit_message>
<xml_diff>
--- a/InputData/elec/GHESLE/Green Hydrogen Electricity Supply Logit Exponent.xlsx
+++ b/InputData/elec/GHESLE/Green Hydrogen Electricity Supply Logit Exponent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\GHESLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FF48C2-6162-49DF-90A3-86F67A1D8447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F6D1AD-05AB-45C8-A56D-A62CCF42C249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -1248,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-20</v>
+        <v>-200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>